<commit_message>
initial data + setting workspace up
</commit_message>
<xml_diff>
--- a/Projet/Groupe 1 - Projet/Membre du groupe.xlsx
+++ b/Projet/Groupe 1 - Projet/Membre du groupe.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\ISEP3_2025\Stats_spatiale\Statistique-Exploratoire-Spatiale\Projet\Groupe 1 - Projet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +21,41 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Prénom</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>KHADIDIATOU</t>
+  </si>
+  <si>
+    <t>COULIBALY</t>
+  </si>
+  <si>
+    <t>NDONG</t>
+  </si>
+  <si>
+    <t>TAMSIR</t>
+  </si>
+  <si>
+    <t>SAMBA</t>
+  </si>
+  <si>
+    <t>DIENG</t>
+  </si>
+  <si>
+    <t>ONANENA AMANA</t>
+  </si>
+  <si>
+    <t>JEANNE DE LA FLECHE</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,7 +109,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -331,12 +371,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>